<commit_message>
Search by faculty added
</commit_message>
<xml_diff>
--- a/src/exports/students.xlsx
+++ b/src/exports/students.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -82,7 +82,7 @@
     <t>Nguyễn Văn A</t>
   </si>
   <si>
-    <t>2001-02-15</t>
+    <t>2025-03-09</t>
   </si>
   <si>
     <t>Nam</t>
@@ -91,202 +91,67 @@
     <t>Cử nhân</t>
   </si>
   <si>
-    <t>nguyenvaa@e5ample.com</t>
-  </si>
-  <si>
-    <t>0952375688</t>
-  </si>
-  <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>Kỹ thuật phần mềm</t>
-  </si>
-  <si>
-    <t>Đang học</t>
-  </si>
-  <si>
-    <t>123, Lê Lợi, Phường 1, Quận 1, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>456, Trần Hưng Đạo, Phường 5, Quận 5, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>789, Nguyễn Trãi, Phường 3, Quận 10, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>CCCD</t>
-  </si>
-  <si>
-    <t>12306889</t>
-  </si>
-  <si>
-    <t>2015-06-20</t>
-  </si>
-  <si>
-    <t>2035-06-20</t>
-  </si>
-  <si>
-    <t>TP. Hồ Chí Minh</t>
+    <t>dangdiennguyen2112@gmail.com</t>
+  </si>
+  <si>
+    <t>03753753751111</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>CNTT</t>
+  </si>
+  <si>
+    <t>K22</t>
+  </si>
+  <si>
+    <t>Nghi hoc</t>
+  </si>
+  <si>
+    <t>1, null, 3, 4, 5, 61</t>
+  </si>
+  <si>
+    <t>1, null, 4, 5, 6, 87</t>
+  </si>
+  <si>
+    <t>1, null, 7, i9, 7, 6</t>
+  </si>
+  <si>
+    <t>CMND</t>
+  </si>
+  <si>
+    <t>00112233576</t>
+  </si>
+  <si>
+    <t>2025-03-13</t>
+  </si>
+  <si>
+    <t>2025-03-08</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Không</t>
   </si>
   <si>
-    <t>Cấp đổi lần 1</t>
-  </si>
-  <si>
-    <t>Trần Thị c</t>
-  </si>
-  <si>
-    <t>2002-08-22</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>Thạc sĩ</t>
-  </si>
-  <si>
-    <t>tranthic@ex6ample.com</t>
-  </si>
-  <si>
-    <t>0979543210</t>
-  </si>
-  <si>
-    <t>Khoa học máy tính</t>
-  </si>
-  <si>
-    <t>Trí tuệ nhân tạo</t>
-  </si>
-  <si>
-    <t>Đã tốt nghiệp</t>
-  </si>
-  <si>
-    <t>99, Điện Biên Phủ, Phường 15, Bình Thạnh, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>111, Nguyễn Văn Cừ, Phường 4, Quận 5, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>222, Dương Bá Trạc, Phường 1, Quận 8, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>987654381</t>
-  </si>
-  <si>
-    <t>2018-12-15</t>
-  </si>
-  <si>
-    <t>2038-12-15</t>
-  </si>
-  <si>
-    <t>Cấp đổi lần 2</t>
-  </si>
-  <si>
-    <t>Lê Hoàng Dũng</t>
-  </si>
-  <si>
-    <t>2000-05-10</t>
-  </si>
-  <si>
-    <t>lehoangdung@example.com</t>
-  </si>
-  <si>
-    <t>0968745210</t>
-  </si>
-  <si>
-    <t>Kinh tế</t>
-  </si>
-  <si>
-    <t>Quản trị kinh doanh</t>
-  </si>
-  <si>
-    <t>55, Lý Thường Kiệt, Phường 7, Quận Tân Bình, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>77, Hùng Vương, Phường 9, Quận 5, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>99, Ngô Quyền, Phường 3, Quận 10, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>456123789</t>
-  </si>
-  <si>
-    <t>2016-09-12</t>
-  </si>
-  <si>
-    <t>2036-09-12</t>
-  </si>
-  <si>
-    <t>Có</t>
-  </si>
-  <si>
-    <t>Mới cấp</t>
-  </si>
-  <si>
-    <t>Phạm Thị Hạnh</t>
-  </si>
-  <si>
-    <t>2003-11-25</t>
-  </si>
-  <si>
-    <t>phamthihanh@example.com</t>
-  </si>
-  <si>
-    <t>0932658741</t>
-  </si>
-  <si>
-    <t>Y Dược</t>
-  </si>
-  <si>
-    <t>Dược học</t>
-  </si>
-  <si>
-    <t>22, Nguyễn Đình Chiểu, Phường 6, Quận 3, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>33, Tô Hiến Thành, Phường 12, Quận 10, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>44, Lạc Long Quân, Phường 8, Quận Tân Bình, TP. Hồ Chí Minh, Việt Nam</t>
-  </si>
-  <si>
-    <t>987321654</t>
-  </si>
-  <si>
-    <t>2019-07-22</t>
-  </si>
-  <si>
-    <t>2039-07-22</t>
-  </si>
-  <si>
     <t>Nguyễn Văn B</t>
   </si>
   <si>
-    <t>nguyenvaa@ex5ample.com</t>
-  </si>
-  <si>
-    <t>0952345688</t>
-  </si>
-  <si>
-    <t>12356889</t>
-  </si>
-  <si>
-    <t>Trần Thị C</t>
-  </si>
-  <si>
-    <t>tranthic@ex5ample.com</t>
-  </si>
-  <si>
-    <t>0976543210</t>
-  </si>
-  <si>
-    <t>987654321</t>
+    <t>dangdiennguyen112@gmail.com</t>
+  </si>
+  <si>
+    <t>0375375375</t>
+  </si>
+  <si>
+    <t>K23</t>
+  </si>
+  <si>
+    <t>00112238576</t>
   </si>
 </sst>
 </file>
@@ -663,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -755,7 +620,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -812,353 +677,81 @@
         <v>39</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="U2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" t="s">
         <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
         <v>35</v>
       </c>
       <c r="P3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="Q3" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="R3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="S3" t="s">
         <v>39</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="U3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" t="s">
         <v>40</v>
-      </c>
-      <c r="V3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>68</v>
-      </c>
-      <c r="R4" t="s">
-        <v>69</v>
-      </c>
-      <c r="S4" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" t="s">
-        <v>70</v>
-      </c>
-      <c r="V4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>78</v>
-      </c>
-      <c r="M5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" t="s">
-        <v>80</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>82</v>
-      </c>
-      <c r="R5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S5" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" t="s">
-        <v>28</v>
-      </c>
-      <c r="U5" t="s">
-        <v>70</v>
-      </c>
-      <c r="V5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" t="s">
-        <v>28</v>
-      </c>
-      <c r="U6" t="s">
-        <v>40</v>
-      </c>
-      <c r="V6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" t="s">
-        <v>51</v>
-      </c>
-      <c r="M7" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" t="s">
-        <v>53</v>
-      </c>
-      <c r="O7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>55</v>
-      </c>
-      <c r="R7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S7" t="s">
-        <v>39</v>
-      </c>
-      <c r="T7" t="s">
-        <v>28</v>
-      </c>
-      <c r="U7" t="s">
-        <v>40</v>
-      </c>
-      <c r="V7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix /more page, student-detail's status
</commit_message>
<xml_diff>
--- a/src/exports/students.xlsx
+++ b/src/exports/students.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -82,46 +82,100 @@
     <t>Nguyễn Văn A</t>
   </si>
   <si>
+    <t>2025-03-01</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>Cử nhân</t>
+  </si>
+  <si>
+    <t>22120001@student.hcmus.edu.vn</t>
+  </si>
+  <si>
+    <t>+84987111222</t>
+  </si>
+  <si>
+    <t>Việt Nam</t>
+  </si>
+  <si>
+    <t>SInh học</t>
+  </si>
+  <si>
+    <t>K21</t>
+  </si>
+  <si>
+    <t>Đang học</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, , , , , </t>
+  </si>
+  <si>
+    <t>1, 2, 34, 5, 7, 8</t>
+  </si>
+  <si>
+    <t>9, 4, 1, 2, 4, 5</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>00112233</t>
+  </si>
+  <si>
+    <t>2025-02-28</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Hoa Kỳ</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Hộ chiếu lưu trú</t>
+  </si>
+  <si>
     <t>2025-03-09</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>Cử nhân</t>
-  </si>
-  <si>
-    <t>dangdiennguyen22@gmail.com</t>
-  </si>
-  <si>
-    <t>0192984211</t>
-  </si>
-  <si>
-    <t>VNam</t>
+    <t>dangdiennguyen2112@gmail.com</t>
+  </si>
+  <si>
+    <t>0375375375</t>
+  </si>
+  <si>
+    <t>VN</t>
   </si>
   <si>
     <t>CNTT</t>
   </si>
   <si>
-    <t>K22</t>
-  </si>
-  <si>
-    <t>Đã tốt nghiệp</t>
-  </si>
-  <si>
-    <t>1234, 1234, 3, 4, Bình Định, 61</t>
-  </si>
-  <si>
-    <t>123443, 1234, 4, Bình Định, Bình Định, 87</t>
-  </si>
-  <si>
-    <t>, 1231, 7, i, 7, 6</t>
-  </si>
-  <si>
-    <t>Passport</t>
-  </si>
-  <si>
-    <t>00112233576</t>
+    <t>K25</t>
+  </si>
+  <si>
+    <t>Nghỉ học</t>
+  </si>
+  <si>
+    <t>1, null, 3, 4, 5, 61</t>
+  </si>
+  <si>
+    <t>1, null, 4, 5, 6, 87</t>
+  </si>
+  <si>
+    <t>1, null, 7, i9, 7, 6</t>
+  </si>
+  <si>
+    <t>CMND</t>
+  </si>
+  <si>
+    <t>204242425645</t>
   </si>
   <si>
     <t>2025-03-13</t>
@@ -133,13 +187,7 @@
     <t>SA</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>Có</t>
-  </si>
-  <si>
-    <t>No comment</t>
+    <t/>
   </si>
   <si>
     <t>Nguyễn Văn B</t>
@@ -148,100 +196,7 @@
     <t>dangdiennguyen112@gmail.com</t>
   </si>
   <si>
-    <t>0375375375</t>
-  </si>
-  <si>
-    <t>VN</t>
-  </si>
-  <si>
-    <t>K23</t>
-  </si>
-  <si>
-    <t>Đã nghỉ học</t>
-  </si>
-  <si>
-    <t>1, 123, 3, 4, HCM, 61</t>
-  </si>
-  <si>
-    <t>1, , 4, 5, 6, 87</t>
-  </si>
-  <si>
-    <t>1, , 7, i, 7, 6</t>
-  </si>
-  <si>
-    <t>CMND</t>
-  </si>
-  <si>
-    <t>00112238576</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Không</t>
-  </si>
-  <si>
-    <t>Trần Lượng</t>
-  </si>
-  <si>
-    <t>2004-03-18</t>
-  </si>
-  <si>
-    <t>CLC</t>
-  </si>
-  <si>
-    <t>luong@gmail.com</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>Hoa hoc</t>
-  </si>
-  <si>
-    <t>Đang học</t>
-  </si>
-  <si>
-    <t>123, null, 4, 5, HCM, VN</t>
-  </si>
-  <si>
-    <t>124, null, 4, 5, HCM, VN</t>
-  </si>
-  <si>
-    <t>125, null, 4, 5, HCM, VN</t>
-  </si>
-  <si>
-    <t>CCCD</t>
-  </si>
-  <si>
-    <t>10001000</t>
-  </si>
-  <si>
-    <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2025-03-18</t>
-  </si>
-  <si>
-    <t>Trịnh Văn G</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>4215454512454157815</t>
-  </si>
-  <si>
-    <t>Trịnh Văn H</t>
-  </si>
-  <si>
-    <t>luong@123.com</t>
-  </si>
-  <si>
-    <t>123412001</t>
-  </si>
-  <si>
-    <t>44541121200</t>
+    <t>772567121</t>
   </si>
 </sst>
 </file>
@@ -618,7 +573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -710,7 +665,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -761,33 +716,33 @@
         <v>37</v>
       </c>
       <c r="R2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
         <v>38</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>41</v>
-      </c>
-      <c r="V2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -802,250 +757,114 @@
         <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q3" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="R3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="T3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="U3" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="V3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
         <v>46</v>
       </c>
       <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s">
         <v>61</v>
       </c>
-      <c r="J4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" t="s">
-        <v>63</v>
-      </c>
-      <c r="M4" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P4" t="s">
-        <v>67</v>
-      </c>
       <c r="Q4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="R4" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="S4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="T4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="U4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>200</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>400</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" t="s">
-        <v>52</v>
-      </c>
-      <c r="P6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" t="s">
-        <v>54</v>
-      </c>
-      <c r="U6" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>